<commit_message>
BG DAN DOWNLOAD TAHAP 1
</commit_message>
<xml_diff>
--- a/public/static/template_table.xlsx
+++ b/public/static/template_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6BD350-9631-4B78-9755-BA79F7B26D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14267BEB-F1C7-4AEB-9B33-1EB0A6312539}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -338,9 +338,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>